<commit_message>
show all missing fields or properties, not just first
in fixture upload
</commit_message>
<xml_diff>
--- a/corehq/apps/fixtures/tests/test_upload/incorrect_fixtures.xlsx
+++ b/corehq/apps/fixtures/tests/test_upload/incorrect_fixtures.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Delete(Y/N)</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>County</t>
+  </si>
+  <si>
+    <t>field 5</t>
+  </si>
+  <si>
+    <t>fun_fact</t>
   </si>
 </sst>
 </file>
@@ -492,24 +498,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,10 +539,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -558,10 +568,13 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -583,11 +596,11 @@
       <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -609,7 +622,7 @@
       <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>